<commit_message>
Auto commit at 2025-09-20 13:20:29.60
</commit_message>
<xml_diff>
--- a/my-page/data/homepage.xlsx
+++ b/my-page/data/homepage.xlsx
@@ -6959,7 +6959,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7079,6 +7079,9 @@
         <v>241255.47000000003</v>
       </c>
       <c r="I12" s="5"/>
+      <c r="J12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" t="s">

</xml_diff>

<commit_message>
Auto commit at 2025-09-20 13:20:52.00
</commit_message>
<xml_diff>
--- a/my-page/data/homepage.xlsx
+++ b/my-page/data/homepage.xlsx
@@ -6959,7 +6959,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7079,9 +7079,6 @@
         <v>241255.47000000003</v>
       </c>
       <c r="I12" s="5"/>
-      <c r="J12">
-        <v>2</v>
-      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" t="s">

</xml_diff>